<commit_message>
done with problem 4 plot
</commit_message>
<xml_diff>
--- a/sol_dengue_data.xlsx
+++ b/sol_dengue_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Orville Hombrebueno\Documents\R\Research_Subject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Orville Hombrebueno\Documents\R\Research_Subject\Dengue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7F78490-2E3F-4C87-90C4-11850DD7F2A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F238E116-2B51-45F7-90FB-0438659ED222}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -150,13 +150,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,7 +499,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
+      <selection activeCell="J2" sqref="J2:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,12 +1116,555 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A108"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A97" sqref="A1:A108"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A102" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A103" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A104" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A106" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A107" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" s="5">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>